<commit_message>
Prepare for final results
</commit_message>
<xml_diff>
--- a/TestData/H_SingleGflInfiniteBus.xlsx
+++ b/TestData/H_SingleGflInfiniteBus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF96680-008B-42C1-BCAA-F9140D15174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E6E72-EBDD-48ED-8C4D-7A96FC399C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -838,10 +838,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H5" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I5" s="2">
         <v>1000</v>
@@ -940,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>